<commit_message>
before 11 th week review
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -26,6 +26,168 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>12/11/2023, 11:02:48 AM</t>
+  </si>
+  <si>
+    <t>sony a7sIII</t>
+  </si>
+  <si>
+    <t>299989.00</t>
+  </si>
+  <si>
+    <t>Canon EF 16-35mm f/2.8L USM Wide Angle Lens</t>
+  </si>
+  <si>
+    <t>85972.00</t>
+  </si>
+  <si>
+    <t>12/11/2023, 11:01:41 AM</t>
+  </si>
+  <si>
+    <t>11/29/2023, 11:50:06 AM</t>
+  </si>
+  <si>
+    <t>FUJIFILM Fuji 35mm f/1.4 XF R Lens</t>
+  </si>
+  <si>
+    <t>59999.00</t>
+  </si>
+  <si>
+    <t>11/29/2023, 10:33:11 AM</t>
+  </si>
+  <si>
+    <t>11/29/2023, 10:33:00 AM</t>
+  </si>
+  <si>
+    <t>11/29/2023, 10:27:02 AM</t>
+  </si>
+  <si>
+    <t>11/29/2023, 10:26:57 AM</t>
+  </si>
+  <si>
+    <t>11/27/2023, 2:48:32 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJI Gimbal for Mobile Phones </t>
+  </si>
+  <si>
+    <t>9000.00</t>
+  </si>
+  <si>
+    <t>11/27/2023, 10:23:10 AM</t>
+  </si>
+  <si>
+    <t>Canon EOS 200D II DSLR Camera EF-S18-55mm IS STM  (Black)</t>
+  </si>
+  <si>
+    <t>58398.00</t>
+  </si>
+  <si>
+    <t>11/27/2023, 10:21:22 AM</t>
+  </si>
+  <si>
+    <t>SanDisk Ultra 32 GB SDHC UHS-I Card Class 10 120 Mbps Memory Card</t>
+  </si>
+  <si>
+    <t>499.00</t>
+  </si>
+  <si>
+    <t>11/27/2023, 10:18:54 AM</t>
+  </si>
+  <si>
+    <t>11/27/2023, 10:07:44 AM</t>
+  </si>
+  <si>
+    <t>171944.00</t>
+  </si>
+  <si>
+    <t>11/27/2023, 10:02:07 AM</t>
+  </si>
+  <si>
+    <t>11/27/2023, 9:52:59 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dron </t>
+  </si>
+  <si>
+    <t>60001.00</t>
+  </si>
+  <si>
+    <t>11/27/2023, 9:51:08 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canon Vlogging Camera For Begners </t>
+  </si>
+  <si>
+    <t>43900.00</t>
+  </si>
+  <si>
+    <t>11/27/2023, 9:45:24 AM</t>
+  </si>
+  <si>
+    <t>Sony FX6</t>
+  </si>
+  <si>
+    <t>599990.00</t>
+  </si>
+  <si>
+    <t>11/27/2023, 9:27:03 AM</t>
+  </si>
+  <si>
+    <t>599978.00</t>
+  </si>
+  <si>
+    <t>11/24/2023, 3:45:15 PM</t>
+  </si>
+  <si>
+    <t>SONY Alpha Full Frame ILCE-7M2K/BQ IN5 Mirrorless Camera Body with 28 - 70 mm Lens  (Black)</t>
+  </si>
+  <si>
+    <t>76990.00</t>
+  </si>
+  <si>
+    <t>11/24/2023, 3:41:18 PM</t>
+  </si>
+  <si>
+    <t>11/23/2023, 8:13:46 PM</t>
+  </si>
+  <si>
+    <t>11/22/2023, 5:26:31 PM</t>
+  </si>
+  <si>
+    <t>alis E88 PRO Drone</t>
+  </si>
+  <si>
+    <t>4999.00</t>
+  </si>
+  <si>
+    <t>11/22/2023, 5:23:51 PM</t>
+  </si>
+  <si>
+    <t>11/22/2023, 2:56:09 PM</t>
+  </si>
+  <si>
+    <t>Universal Addon kit</t>
+  </si>
+  <si>
+    <t>100008.00</t>
+  </si>
+  <si>
+    <t>11/22/2023, 10:49:54 AM</t>
+  </si>
+  <si>
+    <t>FUJIFILM Camera with Fuji 35mm f/1.4 XF R Lens</t>
+  </si>
+  <si>
+    <t>80000.00</t>
+  </si>
+  <si>
+    <t>160000.00</t>
+  </si>
+  <si>
+    <t>11/21/2023, 12:06:10 PM</t>
   </si>
 </sst>
 </file>
@@ -402,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E31"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -422,6 +584,516 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>